<commit_message>
Add Streamlit frontend and update dependencies
</commit_message>
<xml_diff>
--- a/Pagamentos_Excel.xlsx
+++ b/Pagamentos_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gilvanmarques/Library/Mobile Documents/com~apple~CloudDocs/Programação/ConversorPagamentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75437E50-C5EF-724A-A93F-737982B471DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42B1BFC-C3C6-DA40-BFD6-0973960EFD85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="33600" windowHeight="20380" xr2:uid="{1D9981CC-E09D-E149-9D41-1623109E5A49}"/>
+    <workbookView xWindow="13820" yWindow="-20980" windowWidth="25600" windowHeight="20980" xr2:uid="{1D9981CC-E09D-E149-9D41-1623109E5A49}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>id_pagamento</t>
   </si>
@@ -607,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C165183E-6FA2-A34B-8E21-9DD4E4F28A52}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -781,6 +781,51 @@
       <c r="R3" s="5"/>
       <c r="S3" s="8"/>
     </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="6">
+        <v>46078</v>
+      </c>
+      <c r="D4" s="7">
+        <v>30000</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="5">
+        <v>13015151000165</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5">
+        <v>260</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5">
+        <v>123</v>
+      </c>
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5">
+        <v>1</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="8"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F40:F80" xr:uid="{7AB9F4AD-421C-EC41-92C4-34BA6BDD3A4A}">
@@ -805,7 +850,7 @@
           <x14:formula1>
             <xm:f>Planilha2!$F$3:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
+          <xm:sqref>B2:B4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{12CDE083-AA24-0245-8CD3-8C8E09E04EE3}">
           <x14:formula1>

</xml_diff>